<commit_message>
unit test GetKensaGaichu (ConvertConversionItemToOrderInfModel: case 013 - 019)
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/ConvertConversionItemToDetailModelSample.xlsx
+++ b/CloudTest/SampleData/ConvertConversionItemToDetailModelSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LNV\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8372F5-D635-482E-91CB-5FCCBCE316AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB61850-A62B-4EDF-9932-FA9FB53B2765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{2B71D135-FBE3-4021-A4CC-E980BDC61F06}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2B71D135-FBE3-4021-A4CC-E980BDC61F06}"/>
   </bookViews>
   <sheets>
     <sheet name="TenMst" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="245">
   <si>
     <t>HP_ID</t>
   </si>
@@ -756,6 +756,12 @@
   </si>
   <si>
     <t>ipnNameTest</t>
+  </si>
+  <si>
+    <t>ItemCd2</t>
+  </si>
+  <si>
+    <t>testItem2</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A2BDEF-30EB-495C-B277-204C25E3D15F}">
-  <dimension ref="A1:GG3"/>
+  <dimension ref="A1:GG4"/>
   <sheetViews>
-    <sheetView topLeftCell="EK1" workbookViewId="0">
-      <selection activeCell="EQ6" sqref="EQ6"/>
+    <sheetView tabSelected="1" topLeftCell="EA1" workbookViewId="0">
+      <selection activeCell="EZ4" sqref="EZ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2658,6 +2664,488 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:189" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4">
+        <v>20220403</v>
+      </c>
+      <c r="D4">
+        <v>20250331</v>
+      </c>
+      <c r="E4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I4" t="s">
+        <v>193</v>
+      </c>
+      <c r="P4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>12</v>
+      </c>
+      <c r="S4">
+        <v>33</v>
+      </c>
+      <c r="T4" t="s">
+        <v>195</v>
+      </c>
+      <c r="V4" t="s">
+        <v>195</v>
+      </c>
+      <c r="W4" t="s">
+        <v>196</v>
+      </c>
+      <c r="X4" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
+      <c r="BF4">
+        <v>0</v>
+      </c>
+      <c r="BG4">
+        <v>0</v>
+      </c>
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
+        <v>0</v>
+      </c>
+      <c r="BJ4">
+        <v>0</v>
+      </c>
+      <c r="BK4">
+        <v>0</v>
+      </c>
+      <c r="BL4">
+        <v>0</v>
+      </c>
+      <c r="BM4">
+        <v>0</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
+      </c>
+      <c r="BO4">
+        <v>0</v>
+      </c>
+      <c r="BP4">
+        <v>0</v>
+      </c>
+      <c r="BQ4">
+        <v>0</v>
+      </c>
+      <c r="BR4">
+        <v>0</v>
+      </c>
+      <c r="BS4">
+        <v>0</v>
+      </c>
+      <c r="BT4">
+        <v>0</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
+      <c r="BW4">
+        <v>0</v>
+      </c>
+      <c r="BX4">
+        <v>0</v>
+      </c>
+      <c r="BY4">
+        <v>0</v>
+      </c>
+      <c r="BZ4">
+        <v>0</v>
+      </c>
+      <c r="CA4">
+        <v>0</v>
+      </c>
+      <c r="CB4">
+        <v>0</v>
+      </c>
+      <c r="CC4">
+        <v>0</v>
+      </c>
+      <c r="CD4">
+        <v>0</v>
+      </c>
+      <c r="CE4">
+        <v>0</v>
+      </c>
+      <c r="CF4">
+        <v>0</v>
+      </c>
+      <c r="CG4">
+        <v>0</v>
+      </c>
+      <c r="CT4">
+        <v>0</v>
+      </c>
+      <c r="CU4">
+        <v>0</v>
+      </c>
+      <c r="CV4">
+        <v>0</v>
+      </c>
+      <c r="CW4">
+        <v>0</v>
+      </c>
+      <c r="CX4">
+        <v>0</v>
+      </c>
+      <c r="CY4">
+        <v>1</v>
+      </c>
+      <c r="CZ4">
+        <v>1</v>
+      </c>
+      <c r="DA4">
+        <v>0</v>
+      </c>
+      <c r="DB4">
+        <v>2</v>
+      </c>
+      <c r="DC4">
+        <v>0</v>
+      </c>
+      <c r="DD4">
+        <v>0</v>
+      </c>
+      <c r="DE4">
+        <v>0</v>
+      </c>
+      <c r="DF4">
+        <v>0</v>
+      </c>
+      <c r="DG4">
+        <v>0</v>
+      </c>
+      <c r="DH4">
+        <v>0</v>
+      </c>
+      <c r="DJ4">
+        <v>0</v>
+      </c>
+      <c r="DK4">
+        <v>0</v>
+      </c>
+      <c r="DL4">
+        <v>0</v>
+      </c>
+      <c r="DM4">
+        <v>0</v>
+      </c>
+      <c r="DN4">
+        <v>0</v>
+      </c>
+      <c r="DP4">
+        <v>0</v>
+      </c>
+      <c r="DQ4">
+        <v>0</v>
+      </c>
+      <c r="DR4">
+        <v>0</v>
+      </c>
+      <c r="DS4">
+        <v>0</v>
+      </c>
+      <c r="DT4">
+        <v>0</v>
+      </c>
+      <c r="DU4">
+        <v>0</v>
+      </c>
+      <c r="DV4">
+        <v>0</v>
+      </c>
+      <c r="DW4">
+        <v>4923</v>
+      </c>
+      <c r="DY4" t="s">
+        <v>198</v>
+      </c>
+      <c r="DZ4">
+        <v>1</v>
+      </c>
+      <c r="EA4">
+        <v>0</v>
+      </c>
+      <c r="EB4">
+        <v>20210401</v>
+      </c>
+      <c r="EC4">
+        <v>99999999</v>
+      </c>
+      <c r="ED4">
+        <v>0</v>
+      </c>
+      <c r="EE4">
+        <v>0</v>
+      </c>
+      <c r="EF4">
+        <v>0</v>
+      </c>
+      <c r="EG4">
+        <v>0</v>
+      </c>
+      <c r="EH4">
+        <v>0</v>
+      </c>
+      <c r="EI4">
+        <v>0</v>
+      </c>
+      <c r="EJ4">
+        <v>0</v>
+      </c>
+      <c r="EK4">
+        <v>0</v>
+      </c>
+      <c r="EL4">
+        <v>0</v>
+      </c>
+      <c r="EM4">
+        <v>0</v>
+      </c>
+      <c r="EN4">
+        <v>0</v>
+      </c>
+      <c r="EO4">
+        <v>0</v>
+      </c>
+      <c r="EP4" t="s">
+        <v>242</v>
+      </c>
+      <c r="EQ4">
+        <v>0</v>
+      </c>
+      <c r="ER4">
+        <v>0</v>
+      </c>
+      <c r="ES4">
+        <v>0</v>
+      </c>
+      <c r="ET4">
+        <v>0</v>
+      </c>
+      <c r="EU4">
+        <v>0</v>
+      </c>
+      <c r="EV4">
+        <v>0</v>
+      </c>
+      <c r="EW4">
+        <v>0</v>
+      </c>
+      <c r="EX4">
+        <v>61040607912</v>
+      </c>
+      <c r="EY4">
+        <v>0</v>
+      </c>
+      <c r="EZ4" t="s">
+        <v>244</v>
+      </c>
+      <c r="FA4">
+        <v>0</v>
+      </c>
+      <c r="FD4">
+        <v>0</v>
+      </c>
+      <c r="FE4">
+        <v>0</v>
+      </c>
+      <c r="FF4">
+        <v>0</v>
+      </c>
+      <c r="FG4">
+        <v>0</v>
+      </c>
+      <c r="FH4">
+        <v>0</v>
+      </c>
+      <c r="FI4">
+        <v>0</v>
+      </c>
+      <c r="FJ4">
+        <v>0</v>
+      </c>
+      <c r="FK4">
+        <v>0</v>
+      </c>
+      <c r="FL4">
+        <v>0</v>
+      </c>
+      <c r="FM4">
+        <v>0</v>
+      </c>
+      <c r="FN4">
+        <v>0</v>
+      </c>
+      <c r="FO4" t="s">
+        <v>200</v>
+      </c>
+      <c r="FP4">
+        <v>99909</v>
+      </c>
+      <c r="FR4" t="s">
+        <v>200</v>
+      </c>
+      <c r="FS4">
+        <v>99909</v>
+      </c>
+      <c r="FU4">
+        <v>0</v>
+      </c>
+      <c r="FV4">
+        <v>0</v>
+      </c>
+      <c r="FW4">
+        <v>0</v>
+      </c>
+      <c r="FX4">
+        <v>0</v>
+      </c>
+      <c r="FY4">
+        <v>0</v>
+      </c>
+      <c r="FZ4">
+        <v>0</v>
+      </c>
+      <c r="GA4">
+        <v>0</v>
+      </c>
+      <c r="GB4" t="s">
+        <v>196</v>
+      </c>
+      <c r="GC4">
+        <v>0</v>
+      </c>
+      <c r="GD4">
+        <v>0</v>
+      </c>
+      <c r="GE4">
+        <v>0</v>
+      </c>
+      <c r="GF4">
+        <v>0</v>
+      </c>
+      <c r="GG4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2667,7 +3155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA2AC5B-339C-4C6E-9B27-75B5B73CD7DA}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2753,16 +3241,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C6B4C6-7E0A-41FA-BE12-23455ED68544}">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
@@ -2885,6 +3376,9 @@
       <c r="T2">
         <v>331200</v>
       </c>
+      <c r="U2">
+        <v>331200</v>
+      </c>
       <c r="V2">
         <v>0</v>
       </c>
@@ -2901,6 +3395,53 @@
         <v>0</v>
       </c>
       <c r="AC2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>38735</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>38735</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
         <v>0</v>
       </c>
     </row>

</xml_diff>